<commit_message>
[IMP]Customized custom field creation function for csv and excel import
</commit_message>
<xml_diff>
--- a/custom_field_import/static/src/samples/Field Import Sample.xlsx
+++ b/custom_field_import/static/src/samples/Field Import Sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Odoo Servers\Odoo 15.0e\server\custom_addons\custom_field_import\static\src\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62E78A7-F6D2-49EE-8EF9-F5A2DB49CD55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0DE26B-AEF8-41F2-8D1C-3814EFA23A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{FA4B3BD5-F86A-4228-A973-4C43AE6E14FA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Technical Field Name</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Copied</t>
+  </si>
+  <si>
+    <t>Selection Values</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -431,26 +437,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FFF163-5212-47C9-A6BA-7E3798AC39A8}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="47.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,25 +468,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>